<commit_message>
Menyelesaikan pemodelan data Brazil
</commit_message>
<xml_diff>
--- a/Brazil/data/data.xlsx
+++ b/Brazil/data/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axio\Documents\Penelitian\Brazil\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axio\Documents\Project\Penelitian Time Series\Brazil\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6508002-A0B2-48B1-A4A3-5F815ADFACBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD96A136-85F2-4D8A-BE62-54183F4E63A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1000"/>
+  <dimension ref="A1:B993"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B248" sqref="B1:B248"/>
+    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="A248" sqref="A242:XFD248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2294,60 +2294,25 @@
       </c>
     </row>
     <row r="242" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="3">
-        <v>45292</v>
-      </c>
-      <c r="B242" s="5">
-        <v>46844166.671000019</v>
-      </c>
+      <c r="A242" s="3"/>
     </row>
     <row r="243" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="3">
-        <v>45323</v>
-      </c>
-      <c r="B243" s="5">
-        <v>46318627.08109998</v>
-      </c>
+      <c r="A243" s="3"/>
     </row>
     <row r="244" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="3">
-        <v>45352</v>
-      </c>
-      <c r="B244" s="5">
-        <v>47837268.438900009</v>
-      </c>
+      <c r="A244" s="3"/>
     </row>
     <row r="245" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="3">
-        <v>45383</v>
-      </c>
-      <c r="B245" s="5">
-        <v>47350865.659999996</v>
-      </c>
+      <c r="A245" s="3"/>
     </row>
     <row r="246" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="3">
-        <v>45413</v>
-      </c>
-      <c r="B246" s="5">
-        <v>47050366.659999974</v>
-      </c>
+      <c r="A246" s="3"/>
     </row>
     <row r="247" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A247" s="3">
-        <v>45444</v>
-      </c>
-      <c r="B247" s="5">
-        <v>45555739.309900001</v>
-      </c>
+      <c r="A247" s="3"/>
     </row>
     <row r="248" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="3">
-        <v>45474</v>
-      </c>
-      <c r="B248" s="5">
-        <v>44802602.801000021</v>
-      </c>
+      <c r="A248" s="3"/>
     </row>
     <row r="249" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="3"/>
@@ -2487,27 +2452,13 @@
     <row r="294" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="3"/>
     </row>
-    <row r="295" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A295" s="3"/>
-    </row>
-    <row r="296" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A296" s="3"/>
-    </row>
-    <row r="297" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A297" s="3"/>
-    </row>
-    <row r="298" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A298" s="3"/>
-    </row>
-    <row r="299" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A299" s="3"/>
-    </row>
-    <row r="300" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A300" s="3"/>
-    </row>
-    <row r="301" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A301" s="3"/>
-    </row>
+    <row r="295" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="302" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="303" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="304" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3200,13 +3151,6 @@
     <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>